<commit_message>
Modification noms 2 variables + relecture
</commit_message>
<xml_diff>
--- a/selection_finale.xlsx
+++ b/selection_finale.xlsx
@@ -28,7 +28,7 @@
     <t>Stabilité politique</t>
   </si>
   <si>
-    <t>Import volailles (%)</t>
+    <t>Part non importée volailles (%)</t>
   </si>
   <si>
     <t>Protéines animales (%)</t>
@@ -40,7 +40,7 @@
     <t>Prot. de volailles sur prot. animales (%)</t>
   </si>
   <si>
-    <t>Non Pertes (%)</t>
+    <t>Part non perdue (%)</t>
   </si>
   <si>
     <t>Saturation du marché</t>
@@ -570,7 +570,7 @@
         <v>-0.39</v>
       </c>
       <c r="F2">
-        <v>86.83</v>
+        <v>13.17</v>
       </c>
       <c r="G2">
         <v>29.03</v>
@@ -611,7 +611,7 @@
         <v>1.03</v>
       </c>
       <c r="F3">
-        <v>42.86</v>
+        <v>57.14</v>
       </c>
       <c r="G3">
         <v>43.02</v>
@@ -652,7 +652,7 @@
         <v>0.22</v>
       </c>
       <c r="F4">
-        <v>76.40000000000001</v>
+        <v>23.59999999999999</v>
       </c>
       <c r="G4">
         <v>20.64</v>
@@ -693,7 +693,7 @@
         <v>0.78</v>
       </c>
       <c r="F5">
-        <v>120</v>
+        <v>-20</v>
       </c>
       <c r="G5">
         <v>37.07</v>
@@ -734,7 +734,7 @@
         <v>-0.48</v>
       </c>
       <c r="F6">
-        <v>94.55</v>
+        <v>5.450000000000003</v>
       </c>
       <c r="G6">
         <v>44.94</v>
@@ -775,7 +775,7 @@
         <v>-0.13</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>22.13</v>
@@ -816,7 +816,7 @@
         <v>0.18</v>
       </c>
       <c r="F8">
-        <v>97.44</v>
+        <v>2.560000000000002</v>
       </c>
       <c r="G8">
         <v>49.55</v>
@@ -857,7 +857,7 @@
         <v>-0.03</v>
       </c>
       <c r="F9">
-        <v>200</v>
+        <v>-100</v>
       </c>
       <c r="G9">
         <v>28.36</v>
@@ -898,7 +898,7 @@
         <v>0.01</v>
       </c>
       <c r="F10">
-        <v>71.56</v>
+        <v>28.44</v>
       </c>
       <c r="G10">
         <v>23.35</v>
@@ -939,7 +939,7 @@
         <v>-0.67</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>20.39</v>
@@ -980,7 +980,7 @@
         <v>-0.89</v>
       </c>
       <c r="F12">
-        <v>90.81999999999999</v>
+        <v>9.180000000000007</v>
       </c>
       <c r="G12">
         <v>20.64</v>
@@ -1021,7 +1021,7 @@
         <v>-0.46</v>
       </c>
       <c r="F13">
-        <v>23.27</v>
+        <v>76.73</v>
       </c>
       <c r="G13">
         <v>34.74</v>
@@ -1062,7 +1062,7 @@
         <v>-0.8</v>
       </c>
       <c r="F14">
-        <v>78.12</v>
+        <v>21.88</v>
       </c>
       <c r="G14">
         <v>39.87</v>
@@ -1144,7 +1144,7 @@
         <v>0.22</v>
       </c>
       <c r="F16">
-        <v>72.48999999999999</v>
+        <v>27.51000000000001</v>
       </c>
       <c r="G16">
         <v>48.15</v>
@@ -1185,7 +1185,7 @@
         <v>0.01</v>
       </c>
       <c r="F17">
-        <v>88.23999999999999</v>
+        <v>11.76000000000001</v>
       </c>
       <c r="G17">
         <v>29.71</v>
@@ -1226,7 +1226,7 @@
         <v>-0.7</v>
       </c>
       <c r="F18">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="G18">
         <v>26.81</v>
@@ -1267,7 +1267,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="F19">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>39.21</v>
@@ -1308,7 +1308,7 @@
         <v>-0.8</v>
       </c>
       <c r="F20">
-        <v>109.09</v>
+        <v>-9.090000000000003</v>
       </c>
       <c r="G20">
         <v>37.21</v>
@@ -1349,7 +1349,7 @@
         <v>0.87</v>
       </c>
       <c r="F21">
-        <v>103.57</v>
+        <v>-3.569999999999993</v>
       </c>
       <c r="G21">
         <v>36.61</v>
@@ -1390,7 +1390,7 @@
         <v>0.7</v>
       </c>
       <c r="F22">
-        <v>110.53</v>
+        <v>-10.53</v>
       </c>
       <c r="G22">
         <v>49.39</v>
@@ -1431,7 +1431,7 @@
         <v>0.15</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>32.12</v>
@@ -1472,7 +1472,7 @@
         <v>-0.92</v>
       </c>
       <c r="F24">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="G24">
         <v>37.92</v>
@@ -1513,7 +1513,7 @@
         <v>-0.4</v>
       </c>
       <c r="F25">
-        <v>220</v>
+        <v>-120</v>
       </c>
       <c r="G25">
         <v>25.31</v>
@@ -1554,7 +1554,7 @@
         <v>-0.29</v>
       </c>
       <c r="F26">
-        <v>29.63</v>
+        <v>70.37</v>
       </c>
       <c r="G26">
         <v>16.23</v>
@@ -1595,7 +1595,7 @@
         <v>0.97</v>
       </c>
       <c r="F27">
-        <v>133.33</v>
+        <v>-33.33000000000001</v>
       </c>
       <c r="G27">
         <v>41.9</v>
@@ -1636,7 +1636,7 @@
         <v>0.8</v>
       </c>
       <c r="F28">
-        <v>105.1</v>
+        <v>-5.099999999999994</v>
       </c>
       <c r="G28">
         <v>32.07</v>
@@ -1677,7 +1677,7 @@
         <v>0.33</v>
       </c>
       <c r="F29">
-        <v>200</v>
+        <v>-100</v>
       </c>
       <c r="G29">
         <v>28.52</v>

</xml_diff>